<commit_message>
[vikash]add. automatic page by the TDD approach
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006C60A0-D79A-4488-977D-7842DBB2E078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1746391-FD3C-4C23-89E8-1219B8588900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -40,13 +40,22 @@
     <t>adm@yourstore.com</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>exp</t>
+    <t>vikashkumargupta5a7@gmail.com</t>
+  </si>
+  <si>
+    <t>vikash1</t>
+  </si>
+  <si>
+    <t>vikashkumar</t>
+  </si>
+  <si>
+    <t>vikashkumar@gmail.com</t>
+  </si>
+  <si>
+    <t>vik@gmail.com</t>
+  </si>
+  <si>
+    <t>raju</t>
   </si>
 </sst>
 </file>
@@ -107,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -130,12 +139,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,6 +166,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,71 +485,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -535,8 +583,11 @@
     <hyperlink ref="A3" r:id="rId2" xr:uid="{EB480860-584A-43F6-9478-DD4F2553FE6D}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{EB701B42-A320-4932-9568-F231C8F446AB}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{716734F3-6854-43CF-931C-C8D1149FAF15}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{31A9C50A-8BB6-45AF-A1E3-01B3E1E13587}"/>
+    <hyperlink ref="A9" r:id="rId6" xr:uid="{6D284F3B-CAB1-4028-8F58-D099D6484ADE}"/>
+    <hyperlink ref="A10" r:id="rId7" xr:uid="{4632CC93-B45C-4E1A-9319-061ACED41A11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>